<commit_message>
configured the backend for deployment
</commit_message>
<xml_diff>
--- a/backend/students/STUDENT_NUMBERS.xlsx
+++ b/backend/students/STUDENT_NUMBERS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tshepo Mpofu\Desktop\E-Lections\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tshepo Mpofu\Desktop\E-Lections\backend\students\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A99"/>
+  <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,499 +480,895 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>220217426</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="str">
+        <f>RIGHT(A1,3)</f>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>224789840</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B65" si="0">RIGHT(A2,3)</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>230962154</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>231324399</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>251550042</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>042</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>230615187</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>224182643</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>250279248</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>230955956</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>221277147</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>224173296</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>221388984</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>984</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>242396618</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>221633067</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>067</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>221412419</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>231097732</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>242312619</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>223442722</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>230396540</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>241325660</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>224849486</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>231849882</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>882</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>240495600</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>251112800</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>224165064</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>064</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>223648703</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>250517645</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>241693929</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>241898466</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>241342905</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>905</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>232039779</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>779</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>222073065</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>065</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>231636030</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>030</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>251169241</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>241324011</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>011</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>230795037</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>037</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>241504883</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>883</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>231509470</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>250342764</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>764</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>231468960</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>224066287</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>240275627</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>224707495</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>220441768</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>223045553</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>223244955</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>955</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>230182132</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>223374212</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>220354172</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>231031090</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>090</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
         <v>240020947</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>947</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>241594661</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>251219680</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="10">
         <v>230994960</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>230553696</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>696</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>240825040</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>040</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>241416895</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="10">
         <v>241763870</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>870</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>230353697</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>697</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>221709217</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="10">
         <v>230644022</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>022</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>222524407</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>231349804</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>242477154</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>223355137</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="14">
         <v>221438175</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="str">
+        <f t="shared" ref="B66:B99" si="1">RIGHT(A66,3)</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="12">
         <v>223827004</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="str">
+        <f t="shared" si="1"/>
+        <v>004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>241566064</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>064</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="16">
         <v>220605779</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>779</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>240740729</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>729</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>240272458</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>250615299</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>224369751</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>751</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>231965661</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>221479580</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>223104665</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>665</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>222110289</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>250707398</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="10">
         <v>250908660</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="10">
         <v>240914344</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="10">
         <v>242642490</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>490</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>222827736</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>736</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>231608606</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>230934126</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>231669736</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>736</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>240979276</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="16">
         <v>223203922</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>922</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="16">
         <v>223743013</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>013</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>221992563</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>230377553</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>22358812</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>812</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>240912953</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>953</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>224883773</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>773</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>240587483</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>241382060</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>060</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>220272761</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>761</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <v>224807279</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="17">
         <v>222405327</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="10">
         <v>223852220</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>